<commit_message>
update 25053o test kasir
</commit_message>
<xml_diff>
--- a/laporan.xlsx
+++ b/laporan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\kasir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7ADB6E1-2306-465B-AAB9-7A6CC15A852C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE4DA64-6889-44FF-8AD7-1FE8BE490FDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C664331B-736D-4FFC-B4E4-28891A970B64}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2245" uniqueCount="1039">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2341" uniqueCount="1085">
   <si>
     <t>CS/63/250501/0001</t>
   </si>
@@ -3154,6 +3154,144 @@
   </si>
   <si>
     <t>28 Mei 2025, 20:44</t>
+  </si>
+  <si>
+    <t>CS/63/250529/0001</t>
+  </si>
+  <si>
+    <t>29 Mei 2025, 11:24</t>
+  </si>
+  <si>
+    <t>29 Mei 2025, 11:25</t>
+  </si>
+  <si>
+    <t>CS/63/250529/0002</t>
+  </si>
+  <si>
+    <t>29 Mei 2025, 12:40</t>
+  </si>
+  <si>
+    <t>29 Mei 2025, 12:43</t>
+  </si>
+  <si>
+    <t>CS/63/250529/0003</t>
+  </si>
+  <si>
+    <t>29 Mei 2025, 14:21</t>
+  </si>
+  <si>
+    <t>29 Mei 2025, 14:23</t>
+  </si>
+  <si>
+    <t>CS/63/250529/0004</t>
+  </si>
+  <si>
+    <t>29 Mei 2025, 16:07</t>
+  </si>
+  <si>
+    <t>29 Mei 2025, 16:08</t>
+  </si>
+  <si>
+    <t>CS/63/250529/0005</t>
+  </si>
+  <si>
+    <t>29 Mei 2025, 17:39</t>
+  </si>
+  <si>
+    <t>29 Mei 2025, 18:45</t>
+  </si>
+  <si>
+    <t>CS/63/250529/0006</t>
+  </si>
+  <si>
+    <t>29 Mei 2025, 17:47</t>
+  </si>
+  <si>
+    <t>CS/63/250529/0007</t>
+  </si>
+  <si>
+    <t>29 Mei 2025, 18:54</t>
+  </si>
+  <si>
+    <t>29 Mei 2025, 18:56</t>
+  </si>
+  <si>
+    <t>CS/63/250529/0008</t>
+  </si>
+  <si>
+    <t>29 Mei 2025, 19:01</t>
+  </si>
+  <si>
+    <t>29 Mei 2025, 19:52</t>
+  </si>
+  <si>
+    <t>CS/63/250529/0009</t>
+  </si>
+  <si>
+    <t>29 Mei 2025, 19:26</t>
+  </si>
+  <si>
+    <t>CS/63/250529/0010</t>
+  </si>
+  <si>
+    <t>29 Mei 2025, 19:27</t>
+  </si>
+  <si>
+    <t>29 Mei 2025, 19:28</t>
+  </si>
+  <si>
+    <t>CS/63/250529/0011</t>
+  </si>
+  <si>
+    <t>29 Mei 2025, 19:29</t>
+  </si>
+  <si>
+    <t>29 Mei 2025, 19:33</t>
+  </si>
+  <si>
+    <t>CS/63/250529/0012</t>
+  </si>
+  <si>
+    <t>29 Mei 2025, 20:06</t>
+  </si>
+  <si>
+    <t>29 Mei 2025, 20:08</t>
+  </si>
+  <si>
+    <t>CS/63/250529/0013</t>
+  </si>
+  <si>
+    <t>29 Mei 2025, 20:13</t>
+  </si>
+  <si>
+    <t>29 Mei 2025, 20:15</t>
+  </si>
+  <si>
+    <t>CS/63/250529/0014</t>
+  </si>
+  <si>
+    <t>29 Mei 2025, 20:19</t>
+  </si>
+  <si>
+    <t>29 Mei 2025, 20:20</t>
+  </si>
+  <si>
+    <t>CS/63/250529/0015</t>
+  </si>
+  <si>
+    <t>29 Mei 2025, 20:37</t>
+  </si>
+  <si>
+    <t>29 Mei 2025, 21:38</t>
+  </si>
+  <si>
+    <t>CS/63/250529/0016</t>
+  </si>
+  <si>
+    <t>29 Mei 2025, 21:04</t>
+  </si>
+  <si>
+    <t>29 Mei 2025, 21:05</t>
   </si>
 </sst>
 </file>
@@ -3529,10 +3667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77660A0B-93F9-43A9-821D-52A7AEE2A312}">
-  <dimension ref="C2:N374"/>
+  <dimension ref="C2:N393"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A338" workbookViewId="0">
-      <selection activeCell="K366" sqref="K366"/>
+    <sheetView tabSelected="1" topLeftCell="A358" workbookViewId="0">
+      <selection activeCell="D378" sqref="D378:N393"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16843,6 +16981,609 @@
         <v>177000</v>
       </c>
       <c r="N374">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="375" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="L375" t="e">
+        <f>VLOOKUP(K375,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N375">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="376" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="L376" t="e">
+        <f>VLOOKUP(K376,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N376">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="377" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="L377" t="e">
+        <f>VLOOKUP(K377,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N377">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="378" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D378" s="1">
+        <v>45806</v>
+      </c>
+      <c r="E378" t="s">
+        <v>1039</v>
+      </c>
+      <c r="F378" t="s">
+        <v>1040</v>
+      </c>
+      <c r="G378" t="s">
+        <v>1041</v>
+      </c>
+      <c r="H378" t="s">
+        <v>3</v>
+      </c>
+      <c r="I378" t="s">
+        <v>4</v>
+      </c>
+      <c r="J378">
+        <v>76000</v>
+      </c>
+      <c r="K378" t="s">
+        <v>9</v>
+      </c>
+      <c r="L378">
+        <f>VLOOKUP(K378,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="M378">
+        <v>76000</v>
+      </c>
+      <c r="N378">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="379" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D379" s="1">
+        <v>45806</v>
+      </c>
+      <c r="E379" t="s">
+        <v>1042</v>
+      </c>
+      <c r="F379" t="s">
+        <v>1043</v>
+      </c>
+      <c r="G379" t="s">
+        <v>1044</v>
+      </c>
+      <c r="H379" t="s">
+        <v>3</v>
+      </c>
+      <c r="I379" t="s">
+        <v>4</v>
+      </c>
+      <c r="J379">
+        <v>157000</v>
+      </c>
+      <c r="K379" t="s">
+        <v>5</v>
+      </c>
+      <c r="L379">
+        <f>VLOOKUP(K379,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="M379">
+        <v>157000</v>
+      </c>
+      <c r="N379">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="380" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D380" s="1">
+        <v>45806</v>
+      </c>
+      <c r="E380" t="s">
+        <v>1045</v>
+      </c>
+      <c r="F380" t="s">
+        <v>1046</v>
+      </c>
+      <c r="G380" t="s">
+        <v>1047</v>
+      </c>
+      <c r="H380" t="s">
+        <v>3</v>
+      </c>
+      <c r="I380" t="s">
+        <v>4</v>
+      </c>
+      <c r="J380">
+        <v>109000</v>
+      </c>
+      <c r="K380" t="s">
+        <v>5</v>
+      </c>
+      <c r="L380">
+        <f>VLOOKUP(K380,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="M380">
+        <v>109000</v>
+      </c>
+      <c r="N380">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="381" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D381" s="1">
+        <v>45806</v>
+      </c>
+      <c r="E381" t="s">
+        <v>1048</v>
+      </c>
+      <c r="F381" t="s">
+        <v>1049</v>
+      </c>
+      <c r="G381" t="s">
+        <v>1050</v>
+      </c>
+      <c r="H381" t="s">
+        <v>3</v>
+      </c>
+      <c r="I381" t="s">
+        <v>4</v>
+      </c>
+      <c r="J381">
+        <v>98000</v>
+      </c>
+      <c r="K381" t="s">
+        <v>5</v>
+      </c>
+      <c r="L381">
+        <f>VLOOKUP(K381,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="M381">
+        <v>98000</v>
+      </c>
+      <c r="N381">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="382" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D382" s="1">
+        <v>45806</v>
+      </c>
+      <c r="E382" t="s">
+        <v>1051</v>
+      </c>
+      <c r="F382" t="s">
+        <v>1052</v>
+      </c>
+      <c r="G382" t="s">
+        <v>1053</v>
+      </c>
+      <c r="H382" t="s">
+        <v>3</v>
+      </c>
+      <c r="I382" t="s">
+        <v>33</v>
+      </c>
+      <c r="J382">
+        <v>57000</v>
+      </c>
+      <c r="K382" t="s">
+        <v>29</v>
+      </c>
+      <c r="L382">
+        <f>VLOOKUP(K382,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="M382">
+        <v>57000</v>
+      </c>
+      <c r="N382">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="383" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D383" s="1">
+        <v>45806</v>
+      </c>
+      <c r="E383" t="s">
+        <v>1054</v>
+      </c>
+      <c r="F383" t="s">
+        <v>1055</v>
+      </c>
+      <c r="G383" t="s">
+        <v>1053</v>
+      </c>
+      <c r="H383" t="s">
+        <v>3</v>
+      </c>
+      <c r="I383" t="s">
+        <v>4</v>
+      </c>
+      <c r="J383">
+        <v>365000</v>
+      </c>
+      <c r="K383" t="s">
+        <v>5</v>
+      </c>
+      <c r="L383">
+        <f>VLOOKUP(K383,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="M383">
+        <v>365000</v>
+      </c>
+      <c r="N383">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="384" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D384" s="1">
+        <v>45806</v>
+      </c>
+      <c r="E384" t="s">
+        <v>1056</v>
+      </c>
+      <c r="F384" t="s">
+        <v>1057</v>
+      </c>
+      <c r="G384" t="s">
+        <v>1058</v>
+      </c>
+      <c r="H384" t="s">
+        <v>3</v>
+      </c>
+      <c r="I384" t="s">
+        <v>4</v>
+      </c>
+      <c r="J384">
+        <v>160000</v>
+      </c>
+      <c r="K384" t="s">
+        <v>5</v>
+      </c>
+      <c r="L384">
+        <f>VLOOKUP(K384,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="M384">
+        <v>160000</v>
+      </c>
+      <c r="N384">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="385" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D385" s="1">
+        <v>45806</v>
+      </c>
+      <c r="E385" t="s">
+        <v>1059</v>
+      </c>
+      <c r="F385" t="s">
+        <v>1060</v>
+      </c>
+      <c r="G385" t="s">
+        <v>1061</v>
+      </c>
+      <c r="H385" t="s">
+        <v>3</v>
+      </c>
+      <c r="I385" t="s">
+        <v>33</v>
+      </c>
+      <c r="J385">
+        <v>55000</v>
+      </c>
+      <c r="K385" t="s">
+        <v>691</v>
+      </c>
+      <c r="L385">
+        <f>VLOOKUP(K385,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="M385">
+        <v>55000</v>
+      </c>
+      <c r="N385">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="386" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D386" s="1">
+        <v>45806</v>
+      </c>
+      <c r="E386" t="s">
+        <v>1062</v>
+      </c>
+      <c r="F386" t="s">
+        <v>1063</v>
+      </c>
+      <c r="G386" t="s">
+        <v>1063</v>
+      </c>
+      <c r="H386" t="s">
+        <v>3</v>
+      </c>
+      <c r="I386" t="s">
+        <v>4</v>
+      </c>
+      <c r="J386">
+        <v>59000</v>
+      </c>
+      <c r="K386" t="s">
+        <v>9</v>
+      </c>
+      <c r="L386">
+        <f>VLOOKUP(K386,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="M386">
+        <v>59000</v>
+      </c>
+      <c r="N386">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="387" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D387" s="1">
+        <v>45806</v>
+      </c>
+      <c r="E387" t="s">
+        <v>1064</v>
+      </c>
+      <c r="F387" t="s">
+        <v>1065</v>
+      </c>
+      <c r="G387" t="s">
+        <v>1066</v>
+      </c>
+      <c r="H387" t="s">
+        <v>3</v>
+      </c>
+      <c r="I387" t="s">
+        <v>4</v>
+      </c>
+      <c r="J387">
+        <v>52000</v>
+      </c>
+      <c r="K387" t="s">
+        <v>9</v>
+      </c>
+      <c r="L387">
+        <f>VLOOKUP(K387,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="M387">
+        <v>52000</v>
+      </c>
+      <c r="N387">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="388" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D388" s="1">
+        <v>45806</v>
+      </c>
+      <c r="E388" t="s">
+        <v>1067</v>
+      </c>
+      <c r="F388" t="s">
+        <v>1068</v>
+      </c>
+      <c r="G388" t="s">
+        <v>1069</v>
+      </c>
+      <c r="H388" t="s">
+        <v>3</v>
+      </c>
+      <c r="I388" t="s">
+        <v>4</v>
+      </c>
+      <c r="J388">
+        <v>70000</v>
+      </c>
+      <c r="K388" t="s">
+        <v>5</v>
+      </c>
+      <c r="L388">
+        <f>VLOOKUP(K388,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="M388">
+        <v>70000</v>
+      </c>
+      <c r="N388">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="389" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D389" s="1">
+        <v>45806</v>
+      </c>
+      <c r="E389" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F389" t="s">
+        <v>1071</v>
+      </c>
+      <c r="G389" t="s">
+        <v>1072</v>
+      </c>
+      <c r="H389" t="s">
+        <v>3</v>
+      </c>
+      <c r="I389" t="s">
+        <v>4</v>
+      </c>
+      <c r="J389">
+        <v>37000</v>
+      </c>
+      <c r="K389" t="s">
+        <v>9</v>
+      </c>
+      <c r="L389">
+        <f>VLOOKUP(K389,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="M389">
+        <v>37000</v>
+      </c>
+      <c r="N389">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="390" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D390" s="1">
+        <v>45806</v>
+      </c>
+      <c r="E390" t="s">
+        <v>1073</v>
+      </c>
+      <c r="F390" t="s">
+        <v>1074</v>
+      </c>
+      <c r="G390" t="s">
+        <v>1075</v>
+      </c>
+      <c r="H390" t="s">
+        <v>3</v>
+      </c>
+      <c r="I390" t="s">
+        <v>4</v>
+      </c>
+      <c r="J390">
+        <v>41000</v>
+      </c>
+      <c r="K390" t="s">
+        <v>9</v>
+      </c>
+      <c r="L390">
+        <f>VLOOKUP(K390,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="M390">
+        <v>41000</v>
+      </c>
+      <c r="N390">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="391" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D391" s="1">
+        <v>45806</v>
+      </c>
+      <c r="E391" t="s">
+        <v>1076</v>
+      </c>
+      <c r="F391" t="s">
+        <v>1077</v>
+      </c>
+      <c r="G391" t="s">
+        <v>1078</v>
+      </c>
+      <c r="H391" t="s">
+        <v>3</v>
+      </c>
+      <c r="I391" t="s">
+        <v>4</v>
+      </c>
+      <c r="J391">
+        <v>85000</v>
+      </c>
+      <c r="K391" t="s">
+        <v>9</v>
+      </c>
+      <c r="L391">
+        <f>VLOOKUP(K391,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="M391">
+        <v>85000</v>
+      </c>
+      <c r="N391">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="392" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D392" s="1">
+        <v>45806</v>
+      </c>
+      <c r="E392" t="s">
+        <v>1079</v>
+      </c>
+      <c r="F392" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G392" t="s">
+        <v>1081</v>
+      </c>
+      <c r="H392" t="s">
+        <v>3</v>
+      </c>
+      <c r="I392" t="s">
+        <v>4</v>
+      </c>
+      <c r="J392">
+        <v>403000</v>
+      </c>
+      <c r="K392" t="s">
+        <v>746</v>
+      </c>
+      <c r="L392">
+        <f>VLOOKUP(K392,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="M392">
+        <v>403000</v>
+      </c>
+      <c r="N392">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="393" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D393" s="1">
+        <v>45806</v>
+      </c>
+      <c r="E393" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F393" t="s">
+        <v>1083</v>
+      </c>
+      <c r="G393" t="s">
+        <v>1084</v>
+      </c>
+      <c r="H393" t="s">
+        <v>3</v>
+      </c>
+      <c r="I393" t="s">
+        <v>4</v>
+      </c>
+      <c r="J393">
+        <v>58000</v>
+      </c>
+      <c r="K393" t="s">
+        <v>9</v>
+      </c>
+      <c r="L393">
+        <f>VLOOKUP(K393,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="M393">
+        <v>58000</v>
+      </c>
+      <c r="N393">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update 250601 rev void
</commit_message>
<xml_diff>
--- a/laporan.xlsx
+++ b/laporan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\kasir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A64274AC-1BA5-43CB-9E7B-0EF7632548A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DFBABA6-8504-48FD-81FC-062BBD38815C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C664331B-736D-4FFC-B4E4-28891A970B64}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2461" uniqueCount="1139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2683" uniqueCount="1239">
   <si>
     <t>CS/63/250501/0001</t>
   </si>
@@ -3454,6 +3454,306 @@
   </si>
   <si>
     <t>30 Mei 2025, 21:29</t>
+  </si>
+  <si>
+    <t>CS/63/250531/0001</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 11:26</t>
+  </si>
+  <si>
+    <t>CS/63/250531/0002</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 12:27</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 16:14</t>
+  </si>
+  <si>
+    <t>CS/63/250531/0003</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 13:32</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 14:22</t>
+  </si>
+  <si>
+    <t>CS/63/250531/0004</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 13:50</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 13:58</t>
+  </si>
+  <si>
+    <t>CS/63/250531/0005</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 14:02</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 14:04</t>
+  </si>
+  <si>
+    <t>CS/63/250531/0006</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 15:40</t>
+  </si>
+  <si>
+    <t>CS/63/250531/0007</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 15:51</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 15:55</t>
+  </si>
+  <si>
+    <t>CS/63/250531/0008</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 16:41</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 21:27</t>
+  </si>
+  <si>
+    <t>CS/63/250531/0009</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 16:57</t>
+  </si>
+  <si>
+    <t>CS/63/250531/0010</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 16:59</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 17:57</t>
+  </si>
+  <si>
+    <t>CS/63/250531/0011</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 18:33</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 18:36</t>
+  </si>
+  <si>
+    <t>CS/63/250531/0012</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 18:44</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 18:45</t>
+  </si>
+  <si>
+    <t>CS/63/250531/0013</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 18:46</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 18:48</t>
+  </si>
+  <si>
+    <t>CS/63/250531/0014</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 18:49</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 18:51</t>
+  </si>
+  <si>
+    <t>CS/63/250531/0015</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 19:07</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 19:11</t>
+  </si>
+  <si>
+    <t>CS/63/250531/0016</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 19:14</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 19:17</t>
+  </si>
+  <si>
+    <t>CS/63/250531/0017</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 19:28</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 19:30</t>
+  </si>
+  <si>
+    <t>CS/63/250531/0018</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 19:33</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 19:35</t>
+  </si>
+  <si>
+    <t>CS/63/250531/0019</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 19:38</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 19:39</t>
+  </si>
+  <si>
+    <t>CS/63/250531/0020</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 19:40</t>
+  </si>
+  <si>
+    <t>CS/63/250531/0021</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 19:41</t>
+  </si>
+  <si>
+    <t>CS/63/250531/0022</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 19:42</t>
+  </si>
+  <si>
+    <t>CS/63/250531/0023</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 19:45</t>
+  </si>
+  <si>
+    <t>CS/63/250531/0024</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 19:56</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 19:58</t>
+  </si>
+  <si>
+    <t>CS/63/250531/0025</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 19:59</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 20:40</t>
+  </si>
+  <si>
+    <t>CS/63/250531/0026</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 20:01</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 20:03</t>
+  </si>
+  <si>
+    <t>CS/63/250531/0027</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 20:04</t>
+  </si>
+  <si>
+    <t>CS/63/250531/0028</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 20:06</t>
+  </si>
+  <si>
+    <t>CS/63/250531/0029</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 20:07</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 20:09</t>
+  </si>
+  <si>
+    <t>CS/63/250531/0030</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 20:11</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 21:45</t>
+  </si>
+  <si>
+    <t>CS/63/250531/0031</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 20:17</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 20:18</t>
+  </si>
+  <si>
+    <t>CS/63/250531/0032</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 20:27</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 20:28</t>
+  </si>
+  <si>
+    <t>CS/63/250531/0033</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 20:29</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 22:28</t>
+  </si>
+  <si>
+    <t>CS/63/250531/0034</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 20:37</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 21:44</t>
+  </si>
+  <si>
+    <t>CS/63/250531/0035</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 20:49</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 20:50</t>
+  </si>
+  <si>
+    <t>CS/63/250531/0036</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 20:51</t>
+  </si>
+  <si>
+    <t>CS/63/250531/0037</t>
+  </si>
+  <si>
+    <t>31 Mei 2025, 20:52</t>
   </si>
 </sst>
 </file>
@@ -3829,10 +4129,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77660A0B-93F9-43A9-821D-52A7AEE2A312}">
-  <dimension ref="C2:N414"/>
+  <dimension ref="C2:N453"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A384" workbookViewId="0">
-      <selection activeCell="K397" sqref="K397"/>
+    <sheetView tabSelected="1" topLeftCell="A417" workbookViewId="0">
+      <selection activeCell="K425" sqref="K425"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18475,6 +18775,1356 @@
         <v>60000</v>
       </c>
       <c r="N414">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="415" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="L415" t="e">
+        <f>VLOOKUP(K415,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N415">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="416" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="L416" t="e">
+        <f>VLOOKUP(K416,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N416">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="417" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D417" s="1">
+        <v>45808</v>
+      </c>
+      <c r="E417" t="s">
+        <v>1139</v>
+      </c>
+      <c r="F417" t="s">
+        <v>1140</v>
+      </c>
+      <c r="G417" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H417" t="s">
+        <v>3</v>
+      </c>
+      <c r="I417" t="s">
+        <v>4</v>
+      </c>
+      <c r="J417">
+        <v>97000</v>
+      </c>
+      <c r="K417" t="s">
+        <v>9</v>
+      </c>
+      <c r="L417">
+        <f>VLOOKUP(K417,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="M417">
+        <v>97000</v>
+      </c>
+      <c r="N417">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="418" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D418" s="1">
+        <v>45808</v>
+      </c>
+      <c r="E418" t="s">
+        <v>1141</v>
+      </c>
+      <c r="F418" t="s">
+        <v>1142</v>
+      </c>
+      <c r="G418" t="s">
+        <v>1143</v>
+      </c>
+      <c r="H418" t="s">
+        <v>3</v>
+      </c>
+      <c r="I418" t="s">
+        <v>4</v>
+      </c>
+      <c r="J418">
+        <v>40000</v>
+      </c>
+      <c r="K418" t="s">
+        <v>9</v>
+      </c>
+      <c r="L418">
+        <f>VLOOKUP(K418,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="M418">
+        <v>40000</v>
+      </c>
+      <c r="N418">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="419" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D419" s="1">
+        <v>45808</v>
+      </c>
+      <c r="E419" t="s">
+        <v>1144</v>
+      </c>
+      <c r="F419" t="s">
+        <v>1145</v>
+      </c>
+      <c r="G419" t="s">
+        <v>1146</v>
+      </c>
+      <c r="H419" t="s">
+        <v>3</v>
+      </c>
+      <c r="I419" t="s">
+        <v>4</v>
+      </c>
+      <c r="J419">
+        <v>62000</v>
+      </c>
+      <c r="K419" t="s">
+        <v>5</v>
+      </c>
+      <c r="L419">
+        <f>VLOOKUP(K419,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="M419">
+        <v>62000</v>
+      </c>
+      <c r="N419">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="420" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D420" s="1">
+        <v>45808</v>
+      </c>
+      <c r="E420" t="s">
+        <v>1147</v>
+      </c>
+      <c r="F420" t="s">
+        <v>1148</v>
+      </c>
+      <c r="G420" t="s">
+        <v>1149</v>
+      </c>
+      <c r="H420" t="s">
+        <v>3</v>
+      </c>
+      <c r="I420" t="s">
+        <v>33</v>
+      </c>
+      <c r="J420">
+        <v>34000</v>
+      </c>
+      <c r="K420" t="s">
+        <v>29</v>
+      </c>
+      <c r="L420">
+        <f>VLOOKUP(K420,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="M420">
+        <v>34000</v>
+      </c>
+      <c r="N420">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="421" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D421" s="1">
+        <v>45808</v>
+      </c>
+      <c r="E421" t="s">
+        <v>1150</v>
+      </c>
+      <c r="F421" t="s">
+        <v>1151</v>
+      </c>
+      <c r="G421" t="s">
+        <v>1152</v>
+      </c>
+      <c r="H421" t="s">
+        <v>3</v>
+      </c>
+      <c r="I421" t="s">
+        <v>4</v>
+      </c>
+      <c r="J421">
+        <v>126500</v>
+      </c>
+      <c r="K421" t="s">
+        <v>9</v>
+      </c>
+      <c r="L421">
+        <f>VLOOKUP(K421,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="M421">
+        <v>126500</v>
+      </c>
+      <c r="N421">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="422" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D422" s="1">
+        <v>45808</v>
+      </c>
+      <c r="E422" t="s">
+        <v>1153</v>
+      </c>
+      <c r="F422" t="s">
+        <v>1154</v>
+      </c>
+      <c r="G422" t="s">
+        <v>1154</v>
+      </c>
+      <c r="H422" t="s">
+        <v>3</v>
+      </c>
+      <c r="I422" t="s">
+        <v>68</v>
+      </c>
+      <c r="J422">
+        <v>7000</v>
+      </c>
+      <c r="K422" t="s">
+        <v>9</v>
+      </c>
+      <c r="L422">
+        <f>VLOOKUP(K422,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="M422">
+        <v>7000</v>
+      </c>
+      <c r="N422">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="423" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D423" s="1">
+        <v>45808</v>
+      </c>
+      <c r="E423" t="s">
+        <v>1155</v>
+      </c>
+      <c r="F423" t="s">
+        <v>1156</v>
+      </c>
+      <c r="G423" t="s">
+        <v>1157</v>
+      </c>
+      <c r="H423" t="s">
+        <v>3</v>
+      </c>
+      <c r="I423" t="s">
+        <v>68</v>
+      </c>
+      <c r="J423">
+        <v>94000</v>
+      </c>
+      <c r="K423" t="s">
+        <v>5</v>
+      </c>
+      <c r="L423">
+        <f>VLOOKUP(K423,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="M423">
+        <v>94000</v>
+      </c>
+      <c r="N423">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="424" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D424" s="1">
+        <v>45808</v>
+      </c>
+      <c r="E424" t="s">
+        <v>1158</v>
+      </c>
+      <c r="F424" t="s">
+        <v>1159</v>
+      </c>
+      <c r="G424" t="s">
+        <v>1160</v>
+      </c>
+      <c r="H424" t="s">
+        <v>3</v>
+      </c>
+      <c r="I424" t="s">
+        <v>4</v>
+      </c>
+      <c r="J424">
+        <v>7000</v>
+      </c>
+      <c r="K424" t="s">
+        <v>746</v>
+      </c>
+      <c r="L424">
+        <f>VLOOKUP(K424,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="M424">
+        <v>7000</v>
+      </c>
+      <c r="N424">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="425" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D425" s="1">
+        <v>45808</v>
+      </c>
+      <c r="E425" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F425" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G425" t="s">
+        <v>1162</v>
+      </c>
+      <c r="H425" t="s">
+        <v>3</v>
+      </c>
+      <c r="I425" t="s">
+        <v>68</v>
+      </c>
+      <c r="J425">
+        <v>1000</v>
+      </c>
+      <c r="K425" t="s">
+        <v>9</v>
+      </c>
+      <c r="L425">
+        <f>VLOOKUP(K425,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="M425">
+        <v>1000</v>
+      </c>
+      <c r="N425">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="426" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D426" s="1">
+        <v>45808</v>
+      </c>
+      <c r="E426" t="s">
+        <v>1163</v>
+      </c>
+      <c r="F426" t="s">
+        <v>1164</v>
+      </c>
+      <c r="G426" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H426" t="s">
+        <v>3</v>
+      </c>
+      <c r="I426" t="s">
+        <v>4</v>
+      </c>
+      <c r="J426">
+        <v>272000</v>
+      </c>
+      <c r="K426" t="s">
+        <v>5</v>
+      </c>
+      <c r="L426">
+        <f>VLOOKUP(K426,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="M426">
+        <v>272000</v>
+      </c>
+      <c r="N426">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="427" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D427" s="1">
+        <v>45808</v>
+      </c>
+      <c r="E427" t="s">
+        <v>1166</v>
+      </c>
+      <c r="F427" t="s">
+        <v>1167</v>
+      </c>
+      <c r="G427" t="s">
+        <v>1168</v>
+      </c>
+      <c r="H427" t="s">
+        <v>3</v>
+      </c>
+      <c r="I427" t="s">
+        <v>4</v>
+      </c>
+      <c r="J427">
+        <v>82000</v>
+      </c>
+      <c r="K427" t="s">
+        <v>9</v>
+      </c>
+      <c r="L427">
+        <f>VLOOKUP(K427,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="M427">
+        <v>82000</v>
+      </c>
+      <c r="N427">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="428" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D428" s="1">
+        <v>45808</v>
+      </c>
+      <c r="E428" t="s">
+        <v>1169</v>
+      </c>
+      <c r="F428" t="s">
+        <v>1170</v>
+      </c>
+      <c r="G428" t="s">
+        <v>1171</v>
+      </c>
+      <c r="H428" t="s">
+        <v>3</v>
+      </c>
+      <c r="I428" t="s">
+        <v>4</v>
+      </c>
+      <c r="J428">
+        <v>94000</v>
+      </c>
+      <c r="K428" t="s">
+        <v>9</v>
+      </c>
+      <c r="L428">
+        <f>VLOOKUP(K428,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="M428">
+        <v>94000</v>
+      </c>
+      <c r="N428">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="429" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D429" s="1">
+        <v>45808</v>
+      </c>
+      <c r="E429" t="s">
+        <v>1172</v>
+      </c>
+      <c r="F429" t="s">
+        <v>1173</v>
+      </c>
+      <c r="G429" t="s">
+        <v>1174</v>
+      </c>
+      <c r="H429" t="s">
+        <v>3</v>
+      </c>
+      <c r="I429" t="s">
+        <v>4</v>
+      </c>
+      <c r="J429">
+        <v>93000</v>
+      </c>
+      <c r="K429" t="s">
+        <v>9</v>
+      </c>
+      <c r="L429">
+        <f>VLOOKUP(K429,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="M429">
+        <v>93000</v>
+      </c>
+      <c r="N429">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="430" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D430" s="1">
+        <v>45808</v>
+      </c>
+      <c r="E430" t="s">
+        <v>1175</v>
+      </c>
+      <c r="F430" t="s">
+        <v>1176</v>
+      </c>
+      <c r="G430" t="s">
+        <v>1177</v>
+      </c>
+      <c r="H430" t="s">
+        <v>3</v>
+      </c>
+      <c r="I430" t="s">
+        <v>4</v>
+      </c>
+      <c r="J430">
+        <v>35000</v>
+      </c>
+      <c r="K430" t="s">
+        <v>9</v>
+      </c>
+      <c r="L430">
+        <f>VLOOKUP(K430,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="M430">
+        <v>35000</v>
+      </c>
+      <c r="N430">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="431" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D431" s="1">
+        <v>45808</v>
+      </c>
+      <c r="E431" t="s">
+        <v>1178</v>
+      </c>
+      <c r="F431" t="s">
+        <v>1179</v>
+      </c>
+      <c r="G431" t="s">
+        <v>1180</v>
+      </c>
+      <c r="H431" t="s">
+        <v>3</v>
+      </c>
+      <c r="I431" t="s">
+        <v>4</v>
+      </c>
+      <c r="J431">
+        <v>140000</v>
+      </c>
+      <c r="K431" t="s">
+        <v>9</v>
+      </c>
+      <c r="L431">
+        <f>VLOOKUP(K431,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="M431">
+        <v>140000</v>
+      </c>
+      <c r="N431">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="432" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D432" s="1">
+        <v>45808</v>
+      </c>
+      <c r="E432" t="s">
+        <v>1181</v>
+      </c>
+      <c r="F432" t="s">
+        <v>1182</v>
+      </c>
+      <c r="G432" t="s">
+        <v>1183</v>
+      </c>
+      <c r="H432" t="s">
+        <v>3</v>
+      </c>
+      <c r="I432" t="s">
+        <v>4</v>
+      </c>
+      <c r="J432">
+        <v>179000</v>
+      </c>
+      <c r="K432" t="s">
+        <v>5</v>
+      </c>
+      <c r="L432">
+        <f>VLOOKUP(K432,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="M432">
+        <v>179000</v>
+      </c>
+      <c r="N432">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="433" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D433" s="1">
+        <v>45808</v>
+      </c>
+      <c r="E433" t="s">
+        <v>1184</v>
+      </c>
+      <c r="F433" t="s">
+        <v>1185</v>
+      </c>
+      <c r="G433" t="s">
+        <v>1186</v>
+      </c>
+      <c r="H433" t="s">
+        <v>3</v>
+      </c>
+      <c r="I433" t="s">
+        <v>4</v>
+      </c>
+      <c r="J433">
+        <v>103000</v>
+      </c>
+      <c r="K433" t="s">
+        <v>9</v>
+      </c>
+      <c r="L433">
+        <f>VLOOKUP(K433,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="M433">
+        <v>103000</v>
+      </c>
+      <c r="N433">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="434" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D434" s="1">
+        <v>45808</v>
+      </c>
+      <c r="E434" t="s">
+        <v>1187</v>
+      </c>
+      <c r="F434" t="s">
+        <v>1188</v>
+      </c>
+      <c r="G434" t="s">
+        <v>1189</v>
+      </c>
+      <c r="H434" t="s">
+        <v>3</v>
+      </c>
+      <c r="I434" t="s">
+        <v>4</v>
+      </c>
+      <c r="J434">
+        <v>176000</v>
+      </c>
+      <c r="K434" t="s">
+        <v>9</v>
+      </c>
+      <c r="L434">
+        <f>VLOOKUP(K434,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="M434">
+        <v>176000</v>
+      </c>
+      <c r="N434">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="435" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D435" s="1">
+        <v>45808</v>
+      </c>
+      <c r="E435" t="s">
+        <v>1190</v>
+      </c>
+      <c r="F435" t="s">
+        <v>1191</v>
+      </c>
+      <c r="G435" t="s">
+        <v>1192</v>
+      </c>
+      <c r="H435" t="s">
+        <v>3</v>
+      </c>
+      <c r="I435" t="s">
+        <v>4</v>
+      </c>
+      <c r="J435">
+        <v>130000</v>
+      </c>
+      <c r="K435" t="s">
+        <v>9</v>
+      </c>
+      <c r="L435">
+        <f>VLOOKUP(K435,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="M435">
+        <v>130000</v>
+      </c>
+      <c r="N435">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="436" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D436" s="1">
+        <v>45808</v>
+      </c>
+      <c r="E436" t="s">
+        <v>1193</v>
+      </c>
+      <c r="F436" t="s">
+        <v>1194</v>
+      </c>
+      <c r="G436" t="s">
+        <v>1194</v>
+      </c>
+      <c r="H436" t="s">
+        <v>3</v>
+      </c>
+      <c r="I436" t="s">
+        <v>68</v>
+      </c>
+      <c r="J436">
+        <v>4000</v>
+      </c>
+      <c r="K436" t="s">
+        <v>9</v>
+      </c>
+      <c r="L436">
+        <f>VLOOKUP(K436,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="M436">
+        <v>4000</v>
+      </c>
+      <c r="N436">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="437" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D437" s="1">
+        <v>45808</v>
+      </c>
+      <c r="E437" t="s">
+        <v>1195</v>
+      </c>
+      <c r="F437" t="s">
+        <v>1196</v>
+      </c>
+      <c r="G437" t="s">
+        <v>1196</v>
+      </c>
+      <c r="H437" t="s">
+        <v>3</v>
+      </c>
+      <c r="I437" t="s">
+        <v>4</v>
+      </c>
+      <c r="J437">
+        <v>38000</v>
+      </c>
+      <c r="K437" t="s">
+        <v>9</v>
+      </c>
+      <c r="L437">
+        <f>VLOOKUP(K437,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="M437">
+        <v>38000</v>
+      </c>
+      <c r="N437">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="438" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D438" s="1">
+        <v>45808</v>
+      </c>
+      <c r="E438" t="s">
+        <v>1197</v>
+      </c>
+      <c r="F438" t="s">
+        <v>1196</v>
+      </c>
+      <c r="G438" t="s">
+        <v>1198</v>
+      </c>
+      <c r="H438" t="s">
+        <v>3</v>
+      </c>
+      <c r="I438" t="s">
+        <v>4</v>
+      </c>
+      <c r="J438">
+        <v>43000</v>
+      </c>
+      <c r="K438" t="s">
+        <v>9</v>
+      </c>
+      <c r="L438">
+        <f>VLOOKUP(K438,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="M438">
+        <v>43000</v>
+      </c>
+      <c r="N438">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="439" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D439" s="1">
+        <v>45808</v>
+      </c>
+      <c r="E439" t="s">
+        <v>1199</v>
+      </c>
+      <c r="F439" t="s">
+        <v>1198</v>
+      </c>
+      <c r="G439" t="s">
+        <v>1200</v>
+      </c>
+      <c r="H439" t="s">
+        <v>3</v>
+      </c>
+      <c r="I439" t="s">
+        <v>4</v>
+      </c>
+      <c r="J439">
+        <v>62000</v>
+      </c>
+      <c r="K439" t="s">
+        <v>9</v>
+      </c>
+      <c r="L439">
+        <f>VLOOKUP(K439,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="M439">
+        <v>62000</v>
+      </c>
+      <c r="N439">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="440" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D440" s="1">
+        <v>45808</v>
+      </c>
+      <c r="E440" t="s">
+        <v>1201</v>
+      </c>
+      <c r="F440" t="s">
+        <v>1202</v>
+      </c>
+      <c r="G440" t="s">
+        <v>1203</v>
+      </c>
+      <c r="H440" t="s">
+        <v>3</v>
+      </c>
+      <c r="I440" t="s">
+        <v>4</v>
+      </c>
+      <c r="J440">
+        <v>17000</v>
+      </c>
+      <c r="K440" t="s">
+        <v>5</v>
+      </c>
+      <c r="L440">
+        <f>VLOOKUP(K440,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="M440">
+        <v>17000</v>
+      </c>
+      <c r="N440">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="441" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D441" s="1">
+        <v>45808</v>
+      </c>
+      <c r="E441" t="s">
+        <v>1204</v>
+      </c>
+      <c r="F441" t="s">
+        <v>1205</v>
+      </c>
+      <c r="G441" t="s">
+        <v>1206</v>
+      </c>
+      <c r="H441" t="s">
+        <v>3</v>
+      </c>
+      <c r="I441" t="s">
+        <v>4</v>
+      </c>
+      <c r="J441">
+        <v>244000</v>
+      </c>
+      <c r="K441" t="s">
+        <v>9</v>
+      </c>
+      <c r="L441">
+        <f>VLOOKUP(K441,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="M441">
+        <v>244000</v>
+      </c>
+      <c r="N441">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="442" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D442" s="1">
+        <v>45808</v>
+      </c>
+      <c r="E442" t="s">
+        <v>1207</v>
+      </c>
+      <c r="F442" t="s">
+        <v>1208</v>
+      </c>
+      <c r="G442" t="s">
+        <v>1209</v>
+      </c>
+      <c r="H442" t="s">
+        <v>3</v>
+      </c>
+      <c r="I442" t="s">
+        <v>4</v>
+      </c>
+      <c r="J442">
+        <v>143000</v>
+      </c>
+      <c r="K442" t="s">
+        <v>9</v>
+      </c>
+      <c r="L442">
+        <f>VLOOKUP(K442,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="M442">
+        <v>143000</v>
+      </c>
+      <c r="N442">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="443" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D443" s="1">
+        <v>45808</v>
+      </c>
+      <c r="E443" t="s">
+        <v>1210</v>
+      </c>
+      <c r="F443" t="s">
+        <v>1209</v>
+      </c>
+      <c r="G443" t="s">
+        <v>1211</v>
+      </c>
+      <c r="H443" t="s">
+        <v>3</v>
+      </c>
+      <c r="I443" t="s">
+        <v>4</v>
+      </c>
+      <c r="J443">
+        <v>75000</v>
+      </c>
+      <c r="K443" t="s">
+        <v>9</v>
+      </c>
+      <c r="L443">
+        <f>VLOOKUP(K443,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="M443">
+        <v>75000</v>
+      </c>
+      <c r="N443">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="444" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D444" s="1">
+        <v>45808</v>
+      </c>
+      <c r="E444" t="s">
+        <v>1212</v>
+      </c>
+      <c r="F444" t="s">
+        <v>1213</v>
+      </c>
+      <c r="G444" t="s">
+        <v>1213</v>
+      </c>
+      <c r="H444" t="s">
+        <v>3</v>
+      </c>
+      <c r="I444" t="s">
+        <v>4</v>
+      </c>
+      <c r="J444">
+        <v>45000</v>
+      </c>
+      <c r="K444" t="s">
+        <v>9</v>
+      </c>
+      <c r="L444">
+        <f>VLOOKUP(K444,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="M444">
+        <v>45000</v>
+      </c>
+      <c r="N444">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="445" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D445" s="1">
+        <v>45808</v>
+      </c>
+      <c r="E445" t="s">
+        <v>1214</v>
+      </c>
+      <c r="F445" t="s">
+        <v>1215</v>
+      </c>
+      <c r="G445" t="s">
+        <v>1216</v>
+      </c>
+      <c r="H445" t="s">
+        <v>3</v>
+      </c>
+      <c r="I445" t="s">
+        <v>4</v>
+      </c>
+      <c r="J445">
+        <v>58000</v>
+      </c>
+      <c r="K445" t="s">
+        <v>5</v>
+      </c>
+      <c r="L445">
+        <f>VLOOKUP(K445,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="M445">
+        <v>58000</v>
+      </c>
+      <c r="N445">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="446" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D446" s="1">
+        <v>45808</v>
+      </c>
+      <c r="E446" t="s">
+        <v>1217</v>
+      </c>
+      <c r="F446" t="s">
+        <v>1218</v>
+      </c>
+      <c r="G446" t="s">
+        <v>1219</v>
+      </c>
+      <c r="H446" t="s">
+        <v>3</v>
+      </c>
+      <c r="I446" t="s">
+        <v>4</v>
+      </c>
+      <c r="J446">
+        <v>77000</v>
+      </c>
+      <c r="K446" t="s">
+        <v>9</v>
+      </c>
+      <c r="L446">
+        <f>VLOOKUP(K446,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="M446">
+        <v>77000</v>
+      </c>
+      <c r="N446">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="447" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D447" s="1">
+        <v>45808</v>
+      </c>
+      <c r="E447" t="s">
+        <v>1220</v>
+      </c>
+      <c r="F447" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G447" t="s">
+        <v>1222</v>
+      </c>
+      <c r="H447" t="s">
+        <v>3</v>
+      </c>
+      <c r="I447" t="s">
+        <v>4</v>
+      </c>
+      <c r="J447">
+        <v>82000</v>
+      </c>
+      <c r="K447" t="s">
+        <v>9</v>
+      </c>
+      <c r="L447">
+        <f>VLOOKUP(K447,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="M447">
+        <v>82000</v>
+      </c>
+      <c r="N447">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="448" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D448" s="1">
+        <v>45808</v>
+      </c>
+      <c r="E448" t="s">
+        <v>1223</v>
+      </c>
+      <c r="F448" t="s">
+        <v>1224</v>
+      </c>
+      <c r="G448" t="s">
+        <v>1225</v>
+      </c>
+      <c r="H448" t="s">
+        <v>3</v>
+      </c>
+      <c r="I448" t="s">
+        <v>4</v>
+      </c>
+      <c r="J448">
+        <v>102000</v>
+      </c>
+      <c r="K448" t="s">
+        <v>9</v>
+      </c>
+      <c r="L448">
+        <f>VLOOKUP(K448,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="M448">
+        <v>102000</v>
+      </c>
+      <c r="N448">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="449" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D449" s="1">
+        <v>45808</v>
+      </c>
+      <c r="E449" t="s">
+        <v>1226</v>
+      </c>
+      <c r="F449" t="s">
+        <v>1227</v>
+      </c>
+      <c r="G449" t="s">
+        <v>1228</v>
+      </c>
+      <c r="H449" t="s">
+        <v>3</v>
+      </c>
+      <c r="I449" t="s">
+        <v>4</v>
+      </c>
+      <c r="J449">
+        <v>20000</v>
+      </c>
+      <c r="K449" t="s">
+        <v>9</v>
+      </c>
+      <c r="L449">
+        <f>VLOOKUP(K449,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="M449">
+        <v>20000</v>
+      </c>
+      <c r="N449">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="450" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D450" s="1">
+        <v>45808</v>
+      </c>
+      <c r="E450" t="s">
+        <v>1229</v>
+      </c>
+      <c r="F450" t="s">
+        <v>1230</v>
+      </c>
+      <c r="G450" t="s">
+        <v>1231</v>
+      </c>
+      <c r="H450" t="s">
+        <v>3</v>
+      </c>
+      <c r="I450" t="s">
+        <v>4</v>
+      </c>
+      <c r="J450">
+        <v>73000</v>
+      </c>
+      <c r="K450" t="s">
+        <v>9</v>
+      </c>
+      <c r="L450">
+        <f>VLOOKUP(K450,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="M450">
+        <v>73000</v>
+      </c>
+      <c r="N450">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="451" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D451" s="1">
+        <v>45808</v>
+      </c>
+      <c r="E451" t="s">
+        <v>1232</v>
+      </c>
+      <c r="F451" t="s">
+        <v>1233</v>
+      </c>
+      <c r="G451" t="s">
+        <v>1234</v>
+      </c>
+      <c r="H451" t="s">
+        <v>3</v>
+      </c>
+      <c r="I451" t="s">
+        <v>68</v>
+      </c>
+      <c r="J451">
+        <v>10000</v>
+      </c>
+      <c r="K451" t="s">
+        <v>9</v>
+      </c>
+      <c r="L451">
+        <f>VLOOKUP(K451,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="M451">
+        <v>10000</v>
+      </c>
+      <c r="N451">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="452" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D452" s="1">
+        <v>45808</v>
+      </c>
+      <c r="E452" t="s">
+        <v>1235</v>
+      </c>
+      <c r="F452" t="s">
+        <v>1234</v>
+      </c>
+      <c r="G452" t="s">
+        <v>1236</v>
+      </c>
+      <c r="H452" t="s">
+        <v>3</v>
+      </c>
+      <c r="I452" t="s">
+        <v>4</v>
+      </c>
+      <c r="J452">
+        <v>38000</v>
+      </c>
+      <c r="K452" t="s">
+        <v>9</v>
+      </c>
+      <c r="L452">
+        <f>VLOOKUP(K452,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="M452">
+        <v>38000</v>
+      </c>
+      <c r="N452">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="453" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D453" s="1">
+        <v>45808</v>
+      </c>
+      <c r="E453" t="s">
+        <v>1237</v>
+      </c>
+      <c r="F453" t="s">
+        <v>1238</v>
+      </c>
+      <c r="G453" t="s">
+        <v>1238</v>
+      </c>
+      <c r="H453" t="s">
+        <v>3</v>
+      </c>
+      <c r="I453" t="s">
+        <v>4</v>
+      </c>
+      <c r="J453">
+        <v>10000</v>
+      </c>
+      <c r="K453" t="s">
+        <v>9</v>
+      </c>
+      <c r="L453">
+        <f>VLOOKUP(K453,Sheet2!$J$5:$L$17,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="M453">
+        <v>10000</v>
+      </c>
+      <c r="N453">
         <v>0</v>
       </c>
     </row>

</xml_diff>